<commit_message>
support new flexcoil transition format
</commit_message>
<xml_diff>
--- a/app/adp/templates/nomenclatures.xlsx
+++ b/app/adp/templates/nomenclatures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carboni\projects\shupe-carboni\backend\app\adp\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189BE454-8A22-4E54-B704-00F2406DD762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BE4E92-952F-4535-AA92-ECB3AD8B0C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6765" yWindow="1410" windowWidth="21075" windowHeight="17370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HE" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="254">
   <si>
     <t>Carrier CE Series</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>03</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
   <si>
     <t>Series</t>
@@ -602,9 +599,6 @@
     <t>Product Code</t>
   </si>
   <si>
-    <t>Access Port</t>
-  </si>
-  <si>
     <t>A: 10.00"</t>
   </si>
   <si>
@@ -783,6 +777,27 @@
   </si>
   <si>
     <t>Horizontal Side Connection Coils</t>
+  </si>
+  <si>
+    <t>Ref. Detection System</t>
+  </si>
+  <si>
+    <t>R:  Included (Factory Installed)</t>
+  </si>
+  <si>
+    <t>N:  Not Included (Field Installed)</t>
+  </si>
+  <si>
+    <t>R: Right-hand</t>
+  </si>
+  <si>
+    <t>Blank: Left-hand</t>
+  </si>
+  <si>
+    <t>Drain Conn.</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -845,7 +860,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -862,8 +877,14 @@
         <fgColor rgb="FFD9E1F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -936,11 +957,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1034,6 +1066,12 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1342,7 +1380,9 @@
   </sheetPr>
   <dimension ref="B1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1355,12 +1395,12 @@
     <col min="8" max="8" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="31"/>
@@ -1377,7 +1417,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D2" s="2">
         <v>9</v>
@@ -1386,13 +1426,13 @@
         <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G2" s="2">
         <v>175</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" s="2">
         <v>20</v>
@@ -1401,12 +1441,12 @@
         <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -1415,25 +1455,25 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1450,121 +1490,125 @@
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="J5" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>194</v>
+      <c r="K5" s="10" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="J6" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="K6" s="8"/>
+      <c r="K6" s="32" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="K7" s="6"/>
+        <v>213</v>
+      </c>
+      <c r="K7" s="32" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K8" s="17"/>
     </row>
     <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
@@ -1577,16 +1621,16 @@
       <c r="G9" s="7"/>
       <c r="H9" s="6"/>
       <c r="I9" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="9"/>
@@ -1598,13 +1642,13 @@
       <c r="H10" s="6"/>
       <c r="I10" s="7"/>
       <c r="J10" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="9" t="s">
@@ -1622,7 +1666,7 @@
     </row>
     <row r="12" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="9" t="s">
@@ -1638,7 +1682,7 @@
     </row>
     <row r="13" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
@@ -1663,10 +1707,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B1" sqref="B1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,24 +1720,27 @@
     <col min="4" max="4" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
       <c r="I1" s="30"/>
-      <c r="J1" s="31"/>
+      <c r="J1" s="30"/>
       <c r="K1" s="30"/>
-    </row>
-    <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+    </row>
+    <row r="2" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1722,18 +1769,24 @@
         <v>1</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>8</v>
@@ -1742,22 +1795,28 @@
         <v>9</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
@@ -1768,122 +1827,142 @@
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
       <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="8"/>
+      <c r="M6" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="6"/>
       <c r="D7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>64</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>65</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="M7" s="33"/>
+    </row>
+    <row r="8" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="17"/>
-    </row>
-    <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="6"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -1892,12 +1971,14 @@
       <c r="I10" s="6"/>
       <c r="J10" s="9"/>
       <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1906,8 +1987,10 @@
       <c r="I11" s="6"/>
       <c r="J11" s="9"/>
       <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -1918,10 +2001,12 @@
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
       <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1932,11 +2017,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:G13"/>
+  <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1946,19 +2029,21 @@
     <col min="4" max="5" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="2:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+    </row>
+    <row r="2" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1977,8 +2062,11 @@
       <c r="G2" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1997,16 +2085,20 @@
       <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="2:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="6" t="s">
         <v>10</v>
@@ -2023,8 +2115,11 @@
       <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="6" t="s">
         <v>15</v>
@@ -2041,8 +2136,11 @@
       <c r="G6" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="6" t="s">
         <v>20</v>
@@ -2055,8 +2153,9 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="6" t="s">
         <v>23</v>
@@ -2069,8 +2168,9 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="6" t="s">
         <v>26</v>
@@ -2083,8 +2183,9 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="6" t="s">
         <v>29</v>
@@ -2097,8 +2198,9 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7" t="s">
@@ -2107,26 +2209,29 @@
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="6"/>
       <c r="D12" s="9"/>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="12"/>
       <c r="G13" s="13"/>
+      <c r="H13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2137,10 +2242,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:H13"/>
+  <dimension ref="B1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2152,22 +2257,24 @@
     <col min="6" max="6" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" style="14" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+    </row>
+    <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
@@ -2176,19 +2283,22 @@
         <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -2199,19 +2309,22 @@
         <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
@@ -2219,53 +2332,60 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="I6" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>21</v>
@@ -2273,11 +2393,12 @@
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="33"/>
+    </row>
+    <row r="8" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
@@ -2286,11 +2407,12 @@
       <c r="E8" s="7"/>
       <c r="F8" s="6"/>
       <c r="G8" s="10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7" t="s">
@@ -2300,8 +2422,9 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="s">
@@ -2311,8 +2434,9 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="17"/>
+    </row>
+    <row r="11" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="6"/>
       <c r="D11" s="7" t="s">
@@ -2322,8 +2446,9 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="6"/>
       <c r="D12" s="9"/>
@@ -2331,8 +2456,9 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
@@ -2340,10 +2466,11 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
       <c r="H13" s="13"/>
+      <c r="I13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2356,8 +2483,8 @@
   </sheetPr>
   <dimension ref="B1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,12 +2498,12 @@
     <col min="8" max="8" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="31"/>
@@ -2393,7 +2520,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D2" s="2">
         <v>9</v>
@@ -2402,13 +2529,13 @@
         <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G2" s="2">
         <v>175</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" s="2">
         <v>20</v>
@@ -2417,12 +2544,12 @@
         <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -2431,25 +2558,25 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2466,66 +2593,68 @@
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>194</v>
+        <v>244</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>247</v>
-      </c>
-      <c r="K6" s="8"/>
+        <v>245</v>
+      </c>
+      <c r="K6" s="32" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="7" t="s">
@@ -2533,18 +2662,20 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J7" s="16"/>
-      <c r="K7" s="6"/>
+      <c r="K7" s="32" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
@@ -2555,7 +2686,7 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="7"/>
@@ -2564,7 +2695,7 @@
     </row>
     <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
@@ -2582,7 +2713,7 @@
     </row>
     <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="9"/>
@@ -2598,7 +2729,7 @@
     </row>
     <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="9"/>
@@ -2614,7 +2745,7 @@
     </row>
     <row r="12" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="9"/>
@@ -2628,7 +2759,7 @@
     </row>
     <row r="13" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
@@ -2655,7 +2786,9 @@
   </sheetPr>
   <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2666,12 +2799,13 @@
     <col min="7" max="7" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="31"/>
@@ -2688,7 +2822,7 @@
         <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -2697,27 +2831,27 @@
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="2">
         <v>185</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I2" s="2">
         <v>21</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -2726,25 +2860,25 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2761,51 +2895,53 @@
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="H5" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="K5" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="6"/>
       <c r="D6" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="32" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
@@ -2816,12 +2952,14 @@
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="6"/>
+      <c r="K7" s="32" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
@@ -2834,7 +2972,7 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="9"/>
@@ -2852,7 +2990,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="7"/>
@@ -2868,7 +3006,7 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="7"/>
@@ -2914,9 +3052,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:E11"/>
+  <dimension ref="B1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2925,19 +3065,21 @@
     <col min="3" max="3" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" s="31"/>
+        <v>175</v>
+      </c>
+      <c r="C1" s="30"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
-    </row>
-    <row r="2" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+    </row>
+    <row r="2" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2">
         <v>24</v>
@@ -2948,13 +3090,16 @@
       <c r="E2" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -2962,16 +3107,20 @@
       <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>11</v>
@@ -2980,28 +3129,35 @@
         <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="32"/>
+    </row>
+    <row r="8" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="7" t="s">
         <v>24</v>
@@ -3010,8 +3166,9 @@
       <c r="E8" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="7" t="s">
         <v>27</v>
@@ -3020,26 +3177,29 @@
       <c r="E9" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="25"/>
       <c r="C11" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="26"/>
+      <c r="F11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3050,9 +3210,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:G13"/>
+  <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3063,19 +3225,21 @@
     <col min="5" max="5" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="31"/>
+        <v>154</v>
+      </c>
+      <c r="C1" s="30"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+    </row>
+    <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3089,24 +3253,27 @@
         <v>145</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G2" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
@@ -3114,18 +3281,22 @@
       <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>11</v>
@@ -3134,82 +3305,91 @@
         <v>15</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>163</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="G6" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="17"/>
+    </row>
+    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>30</v>
@@ -3218,10 +3398,11 @@
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="17"/>
+    </row>
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>32</v>
@@ -3230,30 +3411,33 @@
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="10"/>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="12"/>
       <c r="G13" s="13"/>
+      <c r="H13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3279,7 +3463,7 @@
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="30"/>
@@ -3287,13 +3471,13 @@
     </row>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2">
         <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" s="2">
         <v>145</v>
@@ -3301,10 +3485,10 @@
     </row>
     <row r="3" spans="2:5" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -3321,16 +3505,16 @@
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>148</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3339,10 +3523,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>150</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3352,7 +3536,7 @@
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3362,7 +3546,7 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3380,7 +3564,7 @@
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3410,9 +3594,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:K16"/>
+  <dimension ref="B1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3424,37 +3610,39 @@
     <col min="9" max="9" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
-    </row>
-    <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+    </row>
+    <row r="2" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="G2" s="2">
         <v>9</v>
@@ -3463,24 +3651,27 @@
         <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K2" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>5</v>
@@ -3492,19 +3683,22 @@
         <v>9</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -3515,80 +3709,88 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="J5" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>125</v>
-      </c>
       <c r="K5" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>127</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="10"/>
       <c r="G6" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="8"/>
       <c r="K6" s="9" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="L6" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="6"/>
       <c r="F7" s="10"/>
       <c r="G7" s="9"/>
       <c r="H7" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="K7" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -3598,15 +3800,16 @@
         <v>14</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -3616,15 +3819,16 @@
         <v>19</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -3634,11 +3838,12 @@
       <c r="H10" s="7"/>
       <c r="I10" s="10"/>
       <c r="J10" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -3649,8 +3854,9 @@
       <c r="I11" s="10"/>
       <c r="J11" s="8"/>
       <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -3660,11 +3866,12 @@
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
       <c r="J12" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L12" s="17"/>
+    </row>
+    <row r="13" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -3674,11 +3881,12 @@
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
       <c r="J13" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -3688,11 +3896,12 @@
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
       <c r="J14" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -3702,11 +3911,12 @@
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
       <c r="J15" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25"/>
       <c r="C16" s="20"/>
       <c r="D16" s="25"/>
@@ -3717,10 +3927,11 @@
       <c r="I16" s="25"/>
       <c r="J16" s="11"/>
       <c r="K16" s="13"/>
+      <c r="L16" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3731,10 +3942,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:J11"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J6"/>
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3748,33 +3959,35 @@
     <col min="8" max="8" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" style="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="30"/>
       <c r="I1" s="30"/>
-      <c r="J1" s="31"/>
-    </row>
-    <row r="2" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+    </row>
+    <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F2" s="2">
         <v>9</v>
@@ -3783,21 +3996,24 @@
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J2" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>5</v>
@@ -3809,19 +4025,22 @@
         <v>9</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="J3" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -3831,62 +4050,69 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="J5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>107</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="J6" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
@@ -3897,11 +4123,12 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="33"/>
+    </row>
+    <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -3914,11 +4141,12 @@
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -3931,11 +4159,12 @@
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -3946,11 +4175,12 @@
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
       <c r="D11" s="19"/>
@@ -3962,10 +4192,11 @@
       <c r="H11" s="21"/>
       <c r="I11" s="22"/>
       <c r="J11" s="13"/>
+      <c r="K11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3976,10 +4207,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:F12"/>
+  <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F8"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3990,23 +4221,25 @@
     <col min="4" max="4" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -4015,12 +4248,15 @@
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -4029,104 +4265,120 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="2:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="2:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="6"/>
       <c r="D6" s="9"/>
       <c r="E6" s="7"/>
       <c r="F6" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="33"/>
+    </row>
+    <row r="8" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="9"/>
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="9"/>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated templates with TXVs
</commit_message>
<xml_diff>
--- a/app/adp/templates/nomenclatures.xlsx
+++ b/app/adp/templates/nomenclatures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carboni\projects\shupe-carboni\backend\app\adp\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BE4E92-952F-4535-AA92-ECB3AD8B0C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997FC4C8-F1D9-44EB-B8BD-34B0AD9E8C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="254">
   <si>
     <t>Carrier CE Series</t>
   </si>
@@ -184,10 +184,6 @@
   </si>
   <si>
     <t>Copper Slab:</t>
-  </si>
-  <si>
-    <t>A: Piston (R410A)
-w/ Access Port</t>
   </si>
   <si>
     <t>H: Horiz. Only</t>
@@ -224,9 +220,6 @@
     <t>Aluminum Slab:</t>
   </si>
   <si>
-    <t>H: Non-bleed HP-A/C TXV (R410A)</t>
-  </si>
-  <si>
     <t>P: Pull disconnect</t>
   </si>
   <si>
@@ -279,10 +272,6 @@
 M6, M7</t>
   </si>
   <si>
-    <t>1: Piston
-(R-410A)</t>
-  </si>
-  <si>
     <t>PSC Motor:
 18, 24, 30, 36</t>
   </si>
@@ -359,9 +348,6 @@
     <t>G, SS, TT, UU: Aluminum</t>
   </si>
   <si>
-    <t>(R-410A)</t>
-  </si>
-  <si>
     <t>B: Circuit Breaker</t>
   </si>
   <si>
@@ -798,6 +784,18 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>A: Non-bleed HP-A/C</t>
+  </si>
+  <si>
+    <t>TXV (R-454B)</t>
+  </si>
+  <si>
+    <t>B: Non-bleed HP-A/C</t>
+  </si>
+  <si>
+    <t>TXV (R-32)</t>
   </si>
 </sst>
 </file>
@@ -884,7 +882,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -968,11 +966,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1061,17 +1124,47 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1378,10 +1471,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:K13"/>
+  <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,25 +1492,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D2" s="2">
         <v>9</v>
@@ -1426,13 +1519,13 @@
         <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G2" s="2">
         <v>175</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I2" s="2">
         <v>20</v>
@@ -1441,12 +1534,12 @@
         <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -1455,25 +1548,25 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1490,129 +1583,129 @@
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>107</v>
-      </c>
+      <c r="D6" s="9"/>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>248</v>
+        <v>205</v>
+      </c>
+      <c r="K6" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="9"/>
       <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="9" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="K7" s="32" t="s">
-        <v>249</v>
+        <v>209</v>
+      </c>
+      <c r="K7" s="30" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
-        <v>214</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="K8" s="17"/>
     </row>
     <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>27</v>
@@ -1621,19 +1714,21 @@
       <c r="G9" s="7"/>
       <c r="H9" s="6"/>
       <c r="I9" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="7" t="s">
         <v>30</v>
       </c>
@@ -1642,17 +1737,17 @@
       <c r="H10" s="6"/>
       <c r="I10" s="7"/>
       <c r="J10" s="16" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="9" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>32</v>
@@ -1665,12 +1760,12 @@
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
-        <v>173</v>
+      <c r="B12" s="34" t="s">
+        <v>169</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="9" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
@@ -1681,18 +1776,34 @@
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="12"/>
+      <c r="B13" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="35"/>
+    </row>
+    <row r="14" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="39"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1710,7 +1821,7 @@
   <dimension ref="B1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M1"/>
+      <selection activeCell="F5" sqref="F5:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,20 +1836,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
     </row>
     <row r="2" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -1772,10 +1883,10 @@
         <v>34</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:13" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1810,10 +1921,10 @@
         <v>46</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1843,97 +1954,101 @@
       <c r="E5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="L5" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="M5" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
+      </c>
+      <c r="M5" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="33" t="s">
-        <v>249</v>
+      <c r="M6" s="31" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="6"/>
       <c r="D7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>63</v>
+      <c r="F7" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="M7" s="33"/>
+        <v>246</v>
+      </c>
+      <c r="M7" s="31"/>
     </row>
     <row r="8" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>250</v>
+      </c>
       <c r="G8" s="6"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="17"/>
@@ -1944,14 +2059,16 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="F9" s="9" t="s">
+        <v>251</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="6"/>
@@ -1962,10 +2079,12 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -1978,10 +2097,12 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>253</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2019,7 +2140,9 @@
   </sheetPr>
   <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2033,15 +2156,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -2063,7 +2186,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2086,7 +2209,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2115,8 +2238,8 @@
       <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="32" t="s">
-        <v>248</v>
+      <c r="H5" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2136,8 +2259,8 @@
       <c r="G6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="33" t="s">
-        <v>249</v>
+      <c r="H6" s="31" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2152,8 +2275,10 @@
         <v>22</v>
       </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="33"/>
+      <c r="G7" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
@@ -2167,8 +2292,10 @@
         <v>25</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="33"/>
+      <c r="G8" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
@@ -2182,7 +2309,9 @@
         <v>28</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2197,7 +2326,9 @@
         <v>31</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="6" t="s">
+        <v>253</v>
+      </c>
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2208,7 +2339,7 @@
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2261,20 +2392,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
@@ -2283,19 +2414,19 @@
         <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>230</v>
-      </c>
       <c r="G2" s="29" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H2" s="2">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2309,7 +2440,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
@@ -2321,7 +2452,7 @@
         <v>45</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2337,55 +2468,55 @@
     <row r="5" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="6" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I5" s="32" t="s">
-        <v>248</v>
+        <v>101</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="6" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" s="33" t="s">
-        <v>249</v>
+        <v>106</v>
+      </c>
+      <c r="I6" s="31" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="6" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>21</v>
@@ -2393,10 +2524,10 @@
       <c r="E7" s="9"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H7" s="9"/>
-      <c r="I7" s="33"/>
+      <c r="I7" s="31"/>
     </row>
     <row r="8" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
@@ -2407,10 +2538,10 @@
       <c r="E8" s="7"/>
       <c r="F8" s="6"/>
       <c r="G8" s="10" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H8" s="9"/>
-      <c r="I8" s="33"/>
+      <c r="I8" s="31"/>
     </row>
     <row r="9" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
@@ -2484,7 +2615,7 @@
   <dimension ref="B1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+      <selection activeCell="D4" sqref="D4:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2502,25 +2633,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D2" s="2">
         <v>9</v>
@@ -2529,13 +2660,13 @@
         <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G2" s="2">
         <v>175</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I2" s="2">
         <v>20</v>
@@ -2544,12 +2675,12 @@
         <v>22</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -2558,31 +2689,33 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
@@ -2593,89 +2726,89 @@
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="9" t="s">
-        <v>101</v>
-      </c>
+      <c r="D5" s="9"/>
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>107</v>
+        <v>210</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="9" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="K6" s="32" t="s">
-        <v>248</v>
+        <v>241</v>
+      </c>
+      <c r="K6" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" s="9"/>
+        <v>160</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="J7" s="16"/>
-      <c r="K7" s="32" t="s">
-        <v>249</v>
+      <c r="K7" s="30" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
@@ -2686,7 +2819,7 @@
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="7"/>
@@ -2695,7 +2828,7 @@
     </row>
     <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="9" t="s">
@@ -2713,10 +2846,12 @@
     </row>
     <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>250</v>
+      </c>
       <c r="E10" s="7" t="s">
         <v>30</v>
       </c>
@@ -2729,10 +2864,12 @@
     </row>
     <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>251</v>
+      </c>
       <c r="E11" s="7" t="s">
         <v>32</v>
       </c>
@@ -2745,10 +2882,12 @@
     </row>
     <row r="12" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
@@ -2759,10 +2898,12 @@
     </row>
     <row r="13" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="40" t="s">
+        <v>253</v>
+      </c>
       <c r="E13" s="13"/>
       <c r="F13" s="12"/>
       <c r="G13" s="13"/>
@@ -2784,10 +2925,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+      <selection activeCell="D8" sqref="D8:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,25 +2945,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -2831,27 +2972,27 @@
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G2" s="2">
         <v>185</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I2" s="2">
         <v>21</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -2860,31 +3001,33 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
+      <c r="D4" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
@@ -2895,70 +3038,70 @@
     </row>
     <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="9" t="s">
-        <v>101</v>
-      </c>
+      <c r="D5" s="9"/>
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="K5" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="6"/>
       <c r="D6" s="9" t="s">
-        <v>107</v>
+        <v>210</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="9"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="32" t="s">
-        <v>248</v>
+      <c r="K6" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="E7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="9"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="32" t="s">
-        <v>249</v>
+      <c r="K7" s="30" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2972,7 +3115,7 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="9"/>
@@ -2990,7 +3133,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="7"/>
@@ -3000,13 +3143,15 @@
     <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>250</v>
+      </c>
       <c r="E10" s="7" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="7"/>
@@ -3016,7 +3161,9 @@
     <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="9" t="s">
+        <v>251</v>
+      </c>
       <c r="E11" s="7" t="s">
         <v>32</v>
       </c>
@@ -3028,16 +3175,32 @@
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="35"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="40" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3055,7 +3218,7 @@
   <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+      <selection activeCell="E6" sqref="E6:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3069,17 +3232,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2">
         <v>24</v>
@@ -3091,7 +3254,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:6" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3099,7 +3262,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -3108,7 +3271,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3120,7 +3283,7 @@
     </row>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>11</v>
@@ -3129,10 +3292,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>248</v>
+        <v>98</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3142,10 +3305,10 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>249</v>
+        <v>14</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3154,8 +3317,10 @@
         <v>21</v>
       </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="32"/>
+      <c r="E7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
@@ -3164,7 +3329,7 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="9" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="F8" s="17"/>
     </row>
@@ -3175,7 +3340,7 @@
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="9" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="F9" s="6"/>
     </row>
@@ -3185,7 +3350,9 @@
         <v>30</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3194,7 +3361,9 @@
         <v>32</v>
       </c>
       <c r="D11" s="12"/>
-      <c r="E11" s="26"/>
+      <c r="E11" s="40" t="s">
+        <v>253</v>
+      </c>
       <c r="F11" s="12"/>
     </row>
   </sheetData>
@@ -3213,7 +3382,7 @@
   <dimension ref="B1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3229,15 +3398,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -3253,27 +3422,27 @@
         <v>145</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G2" s="2">
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:8" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>8</v>
@@ -3282,7 +3451,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3296,7 +3465,7 @@
     </row>
     <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>11</v>
@@ -3305,91 +3474,93 @@
         <v>15</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>248</v>
+        <v>98</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>249</v>
+        <v>14</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="32"/>
+      <c r="G7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="9" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="9" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="H9" s="17"/>
     </row>
     <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>30</v>
@@ -3397,12 +3568,14 @@
       <c r="D10" s="10"/>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="H10" s="17"/>
     </row>
     <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>32</v>
@@ -3410,12 +3583,14 @@
       <c r="D11" s="10"/>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="6" t="s">
+        <v>253</v>
+      </c>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="10"/>
@@ -3426,7 +3601,7 @@
     </row>
     <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="12"/>
@@ -3462,22 +3637,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
+      <c r="B1" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2">
         <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2">
         <v>145</v>
@@ -3485,10 +3660,10 @@
     </row>
     <row r="3" spans="2:5" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -3505,16 +3680,16 @@
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3523,10 +3698,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3536,7 +3711,7 @@
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3546,7 +3721,7 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="28" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3564,7 +3739,7 @@
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3597,7 +3772,7 @@
   <dimension ref="B1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3614,35 +3789,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
     </row>
     <row r="2" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G2" s="2">
         <v>9</v>
@@ -3651,16 +3826,16 @@
         <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K2" s="2">
         <v>3</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:12" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3671,7 +3846,7 @@
         <v>40</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>5</v>
@@ -3683,19 +3858,19 @@
         <v>9</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>45</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3714,97 +3889,99 @@
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="32" t="s">
-        <v>248</v>
+        <v>54</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="10"/>
       <c r="G6" s="9" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="8"/>
       <c r="K6" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="L6" s="33" t="s">
-        <v>249</v>
+        <v>124</v>
+      </c>
+      <c r="L6" s="31" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="6"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="H7" s="7" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="24" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="L7" s="33"/>
+        <v>128</v>
+      </c>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="6"/>
       <c r="F8" s="10"/>
       <c r="G8" s="9" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="6"/>
@@ -3816,14 +3993,14 @@
       <c r="E9" s="6"/>
       <c r="F9" s="10"/>
       <c r="G9" s="9" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="6"/>
@@ -3834,11 +4011,13 @@
       <c r="D10" s="10"/>
       <c r="E10" s="6"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="H10" s="7"/>
       <c r="I10" s="10"/>
       <c r="J10" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="6"/>
@@ -3849,7 +4028,9 @@
       <c r="D11" s="10"/>
       <c r="E11" s="6"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="36" t="s">
+        <v>253</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="10"/>
       <c r="J11" s="8"/>
@@ -3862,11 +4043,11 @@
       <c r="D12" s="10"/>
       <c r="E12" s="6"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="43"/>
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
       <c r="J12" s="24" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="17"/>
@@ -3881,7 +4062,7 @@
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
       <c r="J13" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="17"/>
@@ -3896,7 +4077,7 @@
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
       <c r="J14" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="6"/>
@@ -3911,7 +4092,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
       <c r="J15" s="8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="6"/>
@@ -3945,7 +4126,7 @@
   <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+      <selection activeCell="F5" sqref="F5:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3963,31 +4144,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
     </row>
     <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F2" s="2">
         <v>9</v>
@@ -3996,16 +4177,16 @@
         <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="J2" s="2">
         <v>2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4025,19 +4206,19 @@
         <v>9</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>45</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4054,62 +4235,62 @@
     </row>
     <row r="5" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="F5" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>101</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>248</v>
+        <v>101</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>107</v>
+        <v>14</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="K6" s="33" t="s">
-        <v>249</v>
+        <v>106</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4117,16 +4298,18 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="6"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="G7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J7" s="16"/>
-      <c r="K7" s="33"/>
+      <c r="K7" s="31"/>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
@@ -4134,14 +4317,14 @@
       <c r="D8" s="10"/>
       <c r="E8" s="6"/>
       <c r="F8" s="9" t="s">
-        <v>14</v>
+        <v>250</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J8" s="16"/>
       <c r="K8" s="17"/>
@@ -4152,14 +4335,14 @@
       <c r="D9" s="10"/>
       <c r="E9" s="6"/>
       <c r="F9" s="9" t="s">
-        <v>19</v>
+        <v>251</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="6"/>
@@ -4169,13 +4352,15 @@
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="G10" s="7" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="6"/>
@@ -4185,7 +4370,9 @@
       <c r="C11" s="20"/>
       <c r="D11" s="19"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="40" t="s">
+        <v>253</v>
+      </c>
       <c r="G11" s="13" t="s">
         <v>32</v>
       </c>
@@ -4210,7 +4397,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4225,21 +4412,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -4248,10 +4435,10 @@
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4265,13 +4452,13 @@
         <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4284,62 +4471,64 @@
     </row>
     <row r="5" spans="2:7" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>248</v>
+      <c r="G5" s="30" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>249</v>
+        <v>81</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G7" s="33"/>
+        <v>84</v>
+      </c>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
       <c r="C8" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>19</v>
+        <v>250</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="17"/>
@@ -4347,7 +4536,9 @@
     <row r="9" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>251</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
       <c r="G9" s="17"/>
@@ -4355,7 +4546,9 @@
     <row r="10" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -4363,7 +4556,9 @@
     <row r="11" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="36" t="s">
+        <v>253</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -4371,7 +4566,7 @@
     <row r="12" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="13"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>

</xml_diff>

<commit_message>
updated with new nomenclature tab. why isn't this in S3?
</commit_message>
<xml_diff>
--- a/app/adp/templates/nomenclatures.xlsx
+++ b/app/adp/templates/nomenclatures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carboni\projects\shupe-carboni\backend\app\adp\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5386A9-8C04-4C81-AEE3-A6927489BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7D5485-6FE8-4A13-BD97-F039F25BB9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HE" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,14 @@
     <sheet name="CP" sheetId="10" r:id="rId10"/>
     <sheet name="CE" sheetId="11" r:id="rId11"/>
     <sheet name="CF" sheetId="12" r:id="rId12"/>
+    <sheet name="LS" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="260">
   <si>
     <t>Carrier CF Series</t>
   </si>
@@ -799,6 +800,21 @@
   </si>
   <si>
     <t>22: Left-hand cased multi-pos</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Paint</t>
+  </si>
+  <si>
+    <t>L: Lennox Painted</t>
+  </si>
+  <si>
+    <t>S:Constant Speed Motor</t>
+  </si>
+  <si>
+    <t>32E</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1392,7 @@
   </sheetPr>
   <dimension ref="B1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2496,6 +2512,278 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0917BE-9D12-418C-892D-D4FB80C23804}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="17" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+    </row>
+    <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="2">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="J7" s="19"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" s="19"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="19"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="J10" s="19"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added two options to F-series voltage slot
</commit_message>
<xml_diff>
--- a/app/adp/templates/nomenclatures.xlsx
+++ b/app/adp/templates/nomenclatures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\carboni\projects\shupe-carboni\backend\app\adp\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42FD13E-1017-4655-8825-C96F05531D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8007221-4963-474F-9455-593B43CC3089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26280" yWindow="3630" windowWidth="23415" windowHeight="16410" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="2280" windowWidth="23415" windowHeight="16410" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HE" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="282">
   <si>
     <t>Low Profile Air Handler</t>
   </si>
@@ -896,12 +896,21 @@
   <si>
     <t>20: 20 kW</t>
   </si>
+  <si>
+    <t>3: 120 V, 60 Hz, 1ph. (ECM only)</t>
+  </si>
+  <si>
+    <t>4: 120 V, 60 Hz, 1ph. (PSC only)</t>
+  </si>
+  <si>
+    <t>A: None (R-410A legacy model revision)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -968,6 +977,11 @@
       <sz val="14"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1090,7 +1104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1182,15 +1196,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1220,6 +1225,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1545,18 +1562,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -1887,20 +1904,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -2201,15 +2218,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -2434,16 +2451,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -2652,7 +2669,9 @@
   </sheetPr>
   <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2666,22 +2685,22 @@
     <col min="8" max="8" width="21.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" style="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
     </row>
     <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -2832,7 +2851,9 @@
       <c r="I7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="41" t="s">
+        <v>279</v>
+      </c>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2850,7 +2871,9 @@
       <c r="I8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="12"/>
+      <c r="J8" s="41" t="s">
+        <v>280</v>
+      </c>
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2920,7 +2943,7 @@
   </sheetPr>
   <dimension ref="B1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2937,17 +2960,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
     </row>
     <row r="2" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -3019,119 +3042,119 @@
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="31" t="s">
         <v>264</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="33" t="s">
         <v>267</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="34" t="s">
         <v>268</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="31" t="s">
         <v>269</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="J5" s="37"/>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="34" t="s">
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37" t="s">
+      <c r="E6" s="33"/>
+      <c r="F6" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="37"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="34"/>
     </row>
     <row r="7" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31" t="s">
         <v>274</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37" t="s">
+      <c r="E7" s="33"/>
+      <c r="F7" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="35"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="37"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34" t="s">
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37" t="s">
+      <c r="E8" s="33"/>
+      <c r="F8" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="37"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37" t="s">
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="37"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="34"/>
     </row>
     <row r="10" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="37"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="34"/>
     </row>
     <row r="11" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="41" t="s">
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38" t="s">
         <v>278</v>
       </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="40"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3165,18 +3188,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -3475,18 +3498,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -3760,13 +3783,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -3924,15 +3947,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="31"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -4163,12 +4186,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -4313,19 +4336,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="2:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -4645,7 +4668,9 @@
   </sheetPr>
   <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4662,18 +4687,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -4805,7 +4830,9 @@
       <c r="J6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
@@ -4822,7 +4849,9 @@
       <c r="I7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="41" t="s">
+        <v>279</v>
+      </c>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4840,7 +4869,9 @@
       <c r="I8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="12"/>
+      <c r="J8" s="41" t="s">
+        <v>280</v>
+      </c>
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4924,14 +4955,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">

</xml_diff>